<commit_message>
binary -> xml 로 저장형식 변경.
ㅂ
</commit_message>
<xml_diff>
--- a/Doc/XmlDataDocument_170420_물리공격상향.xlsx
+++ b/Doc/XmlDataDocument_170420_물리공격상향.xlsx
@@ -90,7 +90,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1148" uniqueCount="512">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1153" uniqueCount="512">
   <si>
     <t>hero</t>
   </si>
@@ -2451,7 +2451,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2690,12 +2690,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="10" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -5958,7 +5952,7 @@
   <dimension ref="A1:Q82"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="P3" sqref="P3"/>
+      <selection activeCell="Q5" sqref="Q5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -6077,10 +6071,10 @@
       <c r="O2" s="1" t="s">
         <v>511</v>
       </c>
-      <c r="P2">
-        <v>1</v>
-      </c>
-      <c r="Q2" s="80"/>
+      <c r="P2"/>
+      <c r="Q2" s="76" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="3" spans="1:17">
       <c r="A3" s="1" t="s">
@@ -6124,10 +6118,10 @@
       <c r="O3" s="1" t="s">
         <v>511</v>
       </c>
-      <c r="P3">
-        <v>1</v>
-      </c>
-      <c r="Q3" s="80"/>
+      <c r="P3"/>
+      <c r="Q3" s="77" t="s">
+        <v>257</v>
+      </c>
     </row>
     <row r="4" spans="1:17">
       <c r="A4" s="1" t="s">
@@ -6171,10 +6165,10 @@
       <c r="O4" s="1" t="s">
         <v>511</v>
       </c>
-      <c r="P4">
-        <v>1</v>
-      </c>
-      <c r="Q4" s="80"/>
+      <c r="P4"/>
+      <c r="Q4" s="76" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="5" spans="1:17">
       <c r="A5" s="1" t="s">
@@ -6218,10 +6212,10 @@
       <c r="O5" s="1" t="s">
         <v>511</v>
       </c>
-      <c r="P5">
-        <v>1</v>
-      </c>
-      <c r="Q5" s="80"/>
+      <c r="P5"/>
+      <c r="Q5" s="77" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="6" spans="1:17">
       <c r="A6" s="1" t="s">
@@ -6265,10 +6259,10 @@
       <c r="O6" s="1" t="s">
         <v>511</v>
       </c>
-      <c r="P6">
-        <v>1</v>
-      </c>
-      <c r="Q6" s="81"/>
+      <c r="P6"/>
+      <c r="Q6" s="76" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="7" spans="1:17">
       <c r="A7" s="1" t="s">

</xml_diff>